<commit_message>
Adding Multi Browser execution feature to Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\git\repository2\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C98C449-E17F-4627-96E4-07EEF459B1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238A75A0-0B35-4FB0-9026-99E663008AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Priority</t>
   </si>
@@ -82,7 +82,13 @@
     <t>admin1234</t>
   </si>
   <si>
-    <t>No</t>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -471,20 +477,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D6FDC3-F7E8-4451-9467-692C2528CCAA}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -492,13 +498,16 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -506,23 +515,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Custom Annotations in Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\git\repository2\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238A75A0-0B35-4FB0-9026-99E663008AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD330D2-F1C3-4E65-89A1-EE284C163737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>loginLogOutTest</t>
   </si>
@@ -43,9 +37,6 @@
     <t>To Test Login Logout Functionality with Valid Creds</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>testname</t>
   </si>
   <si>
@@ -61,9 +52,6 @@
     <t>To Test Login Logout Functionality with InValid Creds</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -89,6 +77,12 @@
   </si>
   <si>
     <t>edge</t>
+  </si>
+  <si>
+    <t>leaveFeatureTest</t>
+  </si>
+  <si>
+    <t>To test Leave Feature</t>
   </si>
 </sst>
 </file>
@@ -124,9 +118,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -419,55 +412,48 @@
     <col min="2" max="2" width="44.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -477,10 +463,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D6FDC3-F7E8-4451-9467-692C2528CCAA}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,53 +478,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exception handling and Encoder decoder Implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\git\repository2\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD330D2-F1C3-4E65-89A1-EE284C163737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69047DBA-18E9-4DA4-AC20-2E6722EB7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>loginLogOutTest</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin1234</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -83,6 +77,9 @@
   </si>
   <si>
     <t>To test Leave Feature</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
   </si>
 </sst>
 </file>
@@ -118,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -447,10 +445,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -465,15 +463,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D6FDC3-F7E8-4451-9467-692C2528CCAA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -484,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -501,13 +499,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -518,30 +516,30 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding remote execution feature using docker
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\git\repository2\SeleniumAutomationFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCDFA6F-1303-4EAD-A7D7-5234D537C0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A619F9-1056-459E-822C-2AF5804A34A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,25 +64,25 @@
     <t>browser</t>
   </si>
   <si>
+    <t>leaveFeatureTest</t>
+  </si>
+  <si>
+    <t>To test Leave Feature</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>edge</t>
-  </si>
-  <si>
-    <t>leaveFeatureTest</t>
-  </si>
-  <si>
-    <t>To test Leave Feature</t>
-  </si>
-  <si>
-    <t>YWRtaW4xMjM=</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Admin1</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,7 +432,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -443,18 +443,18 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +467,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,13 +502,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -519,30 +519,30 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>